<commit_message>
implemented functionality to the estimate click
</commit_message>
<xml_diff>
--- a/categorized_dataframes.xlsx
+++ b/categorized_dataframes.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LV" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMDB" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DB" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COST LV" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COST SMDB" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COST DB" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Others" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>

</xml_diff>